<commit_message>
OMG spreadsheet heaven - NOT
</commit_message>
<xml_diff>
--- a/data/2017 carrizo camtrap-veg.xlsx
+++ b/data/2017 carrizo camtrap-veg.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylor\Desktop\carrizo 2017 data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22440" windowHeight="13360"/>
   </bookViews>
   <sheets>
     <sheet name="shrub locations" sheetId="3" r:id="rId1"/>
     <sheet name="shrubs" sheetId="1" r:id="rId2"/>
     <sheet name="annuals" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="30">
   <si>
     <t>date</t>
   </si>
@@ -117,18 +115,31 @@
   <si>
     <t>deerweed</t>
   </si>
-  <si>
-    <t>35. 11537</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,8 +162,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -165,7 +184,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -224,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,7 +286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,16 +473,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>42877</v>
       </c>
@@ -495,7 +522,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>42877</v>
       </c>
@@ -515,7 +542,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>42877</v>
       </c>
@@ -535,7 +562,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>42877</v>
       </c>
@@ -555,7 +582,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>42877</v>
       </c>
@@ -575,7 +602,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>42877</v>
       </c>
@@ -595,7 +622,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>42877</v>
       </c>
@@ -615,7 +642,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>42877</v>
       </c>
@@ -635,7 +662,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>42877</v>
       </c>
@@ -655,7 +682,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>42877</v>
       </c>
@@ -675,7 +702,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>42886</v>
       </c>
@@ -695,7 +722,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>42886</v>
       </c>
@@ -715,7 +742,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>42886</v>
       </c>
@@ -735,7 +762,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>42886</v>
       </c>
@@ -755,7 +782,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>42886</v>
       </c>
@@ -775,7 +802,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>42886</v>
       </c>
@@ -795,7 +822,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>42886</v>
       </c>
@@ -815,7 +842,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>42886</v>
       </c>
@@ -835,7 +862,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>42886</v>
       </c>
@@ -855,7 +882,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>42886</v>
       </c>
@@ -875,7 +902,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>42893</v>
       </c>
@@ -895,7 +922,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>42893</v>
       </c>
@@ -915,7 +942,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>42893</v>
       </c>
@@ -925,8 +952,8 @@
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
-        <v>30</v>
+      <c r="D24">
+        <v>35.115369999999999</v>
       </c>
       <c r="E24">
         <v>119.61993</v>
@@ -935,7 +962,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>42893</v>
       </c>
@@ -955,7 +982,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>42893</v>
       </c>
@@ -975,7 +1002,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>42893</v>
       </c>
@@ -995,7 +1022,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>42893</v>
       </c>
@@ -1015,7 +1042,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>42893</v>
       </c>
@@ -1035,7 +1062,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>42893</v>
       </c>
@@ -1055,7 +1082,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>42893</v>
       </c>
@@ -1077,6 +1104,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1084,17 +1117,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="12" max="12" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1115,7 +1148,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1186,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>42877</v>
       </c>
@@ -1191,7 +1224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>42877</v>
       </c>
@@ -1229,7 +1262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>42877</v>
       </c>
@@ -1267,7 +1300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>42877</v>
       </c>
@@ -1305,7 +1338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>42877</v>
       </c>
@@ -1343,7 +1376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>42877</v>
       </c>
@@ -1381,7 +1414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>42877</v>
       </c>
@@ -1419,7 +1452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>42877</v>
       </c>
@@ -1457,7 +1490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>42877</v>
       </c>
@@ -1495,7 +1528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>42877</v>
       </c>
@@ -1533,7 +1566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>42886</v>
       </c>
@@ -1571,7 +1604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>42886</v>
       </c>
@@ -1609,7 +1642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>42886</v>
       </c>
@@ -1647,7 +1680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>42886</v>
       </c>
@@ -1685,7 +1718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>42886</v>
       </c>
@@ -1723,7 +1756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>42886</v>
       </c>
@@ -1761,7 +1794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>42886</v>
       </c>
@@ -1796,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>42886</v>
       </c>
@@ -1834,7 +1867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>42886</v>
       </c>
@@ -1872,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>42886</v>
       </c>
@@ -1910,7 +1943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>42894</v>
       </c>
@@ -1948,7 +1981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>42894</v>
       </c>
@@ -1986,7 +2019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>42894</v>
       </c>
@@ -2024,7 +2057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>42894</v>
       </c>
@@ -2062,7 +2095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>42894</v>
       </c>
@@ -2100,7 +2133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>42894</v>
       </c>
@@ -2138,7 +2171,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>42894</v>
       </c>
@@ -2176,7 +2209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>42894</v>
       </c>
@@ -2214,7 +2247,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>42894</v>
       </c>
@@ -2252,7 +2285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>42894</v>
       </c>
@@ -2298,6 +2331,11 @@
     <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2305,17 +2343,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
@@ -2327,7 +2365,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2371,7 +2409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>42877</v>
       </c>
@@ -2397,7 +2435,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>42877</v>
       </c>
@@ -2423,7 +2461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>42877</v>
       </c>
@@ -2449,7 +2487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>42877</v>
       </c>
@@ -2481,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>42877</v>
       </c>
@@ -2507,7 +2545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>42877</v>
       </c>
@@ -2536,7 +2574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>42877</v>
       </c>
@@ -2562,7 +2600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>42877</v>
       </c>
@@ -2591,7 +2629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>42877</v>
       </c>
@@ -2617,7 +2655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>42877</v>
       </c>
@@ -2646,7 +2684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>42877</v>
       </c>
@@ -2672,7 +2710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>42877</v>
       </c>
@@ -2701,7 +2739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>42877</v>
       </c>
@@ -2730,7 +2768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>42877</v>
       </c>
@@ -2759,7 +2797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>42877</v>
       </c>
@@ -2785,7 +2823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="1">
         <v>42877</v>
       </c>
@@ -2811,7 +2849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>42877</v>
       </c>
@@ -2834,7 +2872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="1">
         <v>42877</v>
       </c>
@@ -2860,7 +2898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1">
         <v>42877</v>
       </c>
@@ -2886,7 +2924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1">
         <v>42877</v>
       </c>
@@ -2909,7 +2947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1">
         <v>42886</v>
       </c>
@@ -2929,7 +2967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1">
         <v>42886</v>
       </c>
@@ -2952,7 +2990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1">
         <v>42886</v>
       </c>
@@ -2981,7 +3019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1">
         <v>42886</v>
       </c>
@@ -3001,7 +3039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1">
         <v>42886</v>
       </c>
@@ -3030,7 +3068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1">
         <v>42886</v>
       </c>
@@ -3056,7 +3094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="1">
         <v>42886</v>
       </c>
@@ -3085,7 +3123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1">
         <v>42886</v>
       </c>
@@ -3108,7 +3146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="1">
         <v>42886</v>
       </c>
@@ -3137,7 +3175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="1">
         <v>42886</v>
       </c>
@@ -3166,7 +3204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="1">
         <v>42886</v>
       </c>
@@ -3192,7 +3230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="1">
         <v>42886</v>
       </c>
@@ -3218,7 +3256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="1">
         <v>42886</v>
       </c>
@@ -3247,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="1">
         <v>42886</v>
       </c>
@@ -3276,7 +3314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="1">
         <v>42886</v>
       </c>
@@ -3302,7 +3340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="1">
         <v>42886</v>
       </c>
@@ -3328,7 +3366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="1">
         <v>42886</v>
       </c>
@@ -3354,7 +3392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="1">
         <v>42886</v>
       </c>
@@ -3389,7 +3427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" s="1">
         <v>42886</v>
       </c>
@@ -3418,7 +3456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="1">
         <v>42886</v>
       </c>
@@ -3444,7 +3482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="1">
         <v>42894</v>
       </c>
@@ -3470,7 +3508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="1">
         <v>42894</v>
       </c>
@@ -3493,7 +3531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="1">
         <v>42894</v>
       </c>
@@ -3519,7 +3557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="1">
         <v>42894</v>
       </c>
@@ -3548,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" s="1">
         <v>42894</v>
       </c>
@@ -3577,7 +3615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" s="1">
         <v>42894</v>
       </c>
@@ -3603,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="1">
         <v>42894</v>
       </c>
@@ -3635,7 +3673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="1">
         <v>42894</v>
       </c>
@@ -3664,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="1">
         <v>42894</v>
       </c>
@@ -3696,7 +3734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="1">
         <v>42894</v>
       </c>
@@ -3725,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="1">
         <v>42894</v>
       </c>
@@ -3754,7 +3792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="1">
         <v>42894</v>
       </c>
@@ -3780,7 +3818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="1">
         <v>42894</v>
       </c>
@@ -3812,7 +3850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="1">
         <v>42894</v>
       </c>
@@ -3838,7 +3876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="1">
         <v>42894</v>
       </c>
@@ -3864,7 +3902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="1">
         <v>42894</v>
       </c>
@@ -3890,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="1">
         <v>42894</v>
       </c>
@@ -3922,7 +3960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="1">
         <v>42894</v>
       </c>
@@ -3945,7 +3983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="1">
         <v>42894</v>
       </c>
@@ -3974,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="1">
         <v>42894</v>
       </c>
@@ -4002,5 +4040,10 @@
     <mergeCell ref="F1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data tidy up complete in sheets
</commit_message>
<xml_diff>
--- a/data/2017 carrizo camtrap-veg.xlsx
+++ b/data/2017 carrizo camtrap-veg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22440" windowHeight="13360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22440" windowHeight="13360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="shrub locations" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="29">
   <si>
     <t>date</t>
   </si>
@@ -110,9 +110,6 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>species and abundance</t>
-  </si>
-  <si>
     <t>deerweed</t>
   </si>
 </sst>
@@ -162,8 +159,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -184,15 +187,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1118,7 +1127,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D3" sqref="D3:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2331,6 +2340,7 @@
     <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2341,10 +2351,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2354,59 +2364,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="F1" s="4" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
+      <c r="A2" s="1">
+        <v>42877</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>65</v>
+      </c>
+      <c r="F2">
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -2420,19 +2444,19 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F3">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2443,22 +2467,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="J4">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2472,19 +2496,25 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F5">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2495,28 +2525,22 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F6">
-        <v>22</v>
-      </c>
-      <c r="G6">
-        <v>45</v>
-      </c>
-      <c r="J6">
-        <v>11</v>
-      </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2530,18 +2554,21 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>29</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="M7">
         <v>4</v>
       </c>
     </row>
@@ -2553,25 +2580,22 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="F8">
-        <v>29</v>
-      </c>
-      <c r="G8">
-        <v>29</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2585,19 +2609,22 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E9">
-        <v>70</v>
-      </c>
-      <c r="F9">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>12</v>
-      </c>
-      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>5</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -2608,25 +2635,22 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>25</v>
-      </c>
-      <c r="G10">
-        <v>25</v>
+        <v>85</v>
+      </c>
+      <c r="F10">
+        <v>17</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="J10">
+        <v>17</v>
+      </c>
+      <c r="I10">
         <v>5</v>
-      </c>
-      <c r="K10">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -2640,19 +2664,22 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E11">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="F11">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="H11">
-        <v>17</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -2663,25 +2690,22 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F12">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H12">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>9</v>
-      </c>
-      <c r="L12">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -2695,18 +2719,21 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="F13">
-        <v>54</v>
-      </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-      <c r="I13">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>28</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
         <v>7</v>
       </c>
     </row>
@@ -2718,25 +2745,25 @@
         <v>1</v>
       </c>
       <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
         <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>40</v>
-      </c>
-      <c r="F14">
-        <v>31</v>
-      </c>
-      <c r="G14">
-        <v>28</v>
-      </c>
-      <c r="J14">
-        <v>12</v>
-      </c>
-      <c r="K14">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -2750,22 +2777,22 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F15">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -2776,25 +2803,22 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F16">
-        <v>27</v>
-      </c>
-      <c r="G16">
-        <v>31</v>
-      </c>
-      <c r="J16">
-        <v>9</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -2808,19 +2832,19 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F17">
-        <v>11</v>
-      </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="G17">
+        <v>19</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -2831,22 +2855,19 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F18">
-        <v>35</v>
-      </c>
-      <c r="G18">
-        <v>19</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -2860,16 +2881,19 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F19">
-        <v>15</v>
-      </c>
-      <c r="I19">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="G19">
+        <v>16</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -2880,22 +2904,22 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="F20">
-        <v>39</v>
-      </c>
-      <c r="G20">
-        <v>16</v>
-      </c>
-      <c r="J20">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -2909,42 +2933,36 @@
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E21">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <v>6</v>
-      </c>
-      <c r="I21">
-        <v>8</v>
+        <v>51</v>
+      </c>
+      <c r="G21">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="1">
-        <v>42877</v>
+        <v>42886</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>60</v>
-      </c>
-      <c r="F22">
-        <v>51</v>
-      </c>
-      <c r="G22">
-        <v>31</v>
+        <v>70</v>
+      </c>
+      <c r="I22">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -2958,13 +2976,16 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E23">
-        <v>70</v>
-      </c>
-      <c r="I23">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="F23">
+        <v>17</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -2975,19 +2996,25 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F24">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G24">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -3001,22 +3028,13 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E25">
         <v>40</v>
       </c>
-      <c r="F25">
-        <v>27</v>
-      </c>
       <c r="G25">
-        <v>7</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="L25">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -3027,16 +3045,25 @@
         <v>2</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -3050,22 +3077,19 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E27">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <v>7</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -3076,22 +3100,25 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>75</v>
-      </c>
-      <c r="F28">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="G28">
-        <v>21</v>
-      </c>
-      <c r="M28">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>14</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -3105,22 +3132,16 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E29">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>14</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -3131,19 +3152,25 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G30">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="H30">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>22</v>
+      </c>
+      <c r="J30">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -3157,22 +3184,22 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E31">
-        <v>90</v>
+        <v>70</v>
+      </c>
+      <c r="F31">
+        <v>18</v>
       </c>
       <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <v>22</v>
-      </c>
-      <c r="J31">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -3183,25 +3210,22 @@
         <v>2</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E32">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F32">
-        <v>18</v>
-      </c>
-      <c r="G32">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>17</v>
       </c>
       <c r="L32">
         <v>1</v>
-      </c>
-      <c r="M32">
-        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -3215,16 +3239,16 @@
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E33">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="F33">
-        <v>7</v>
-      </c>
-      <c r="I33">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <v>33</v>
       </c>
       <c r="L33">
         <v>1</v>
@@ -3238,21 +3262,24 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F34">
         <v>22</v>
       </c>
       <c r="G34">
-        <v>33</v>
-      </c>
-      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="M34">
         <v>1</v>
       </c>
     </row>
@@ -3267,22 +3294,22 @@
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E35">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F35">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="I35">
-        <v>4</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -3293,24 +3320,21 @@
         <v>2</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F36">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G36">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="L36">
         <v>2</v>
       </c>
     </row>
@@ -3325,19 +3349,19 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E37">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F37">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G37">
-        <v>14</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="L37">
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -3348,22 +3372,22 @@
         <v>2</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E38">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F38">
-        <v>26</v>
-      </c>
-      <c r="G38">
-        <v>27</v>
-      </c>
-      <c r="L38">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>9</v>
+      </c>
+      <c r="I38">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -3377,19 +3401,28 @@
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E39">
         <v>60</v>
       </c>
       <c r="F39">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="G39">
+        <v>18</v>
       </c>
       <c r="H39">
-        <v>9</v>
-      </c>
-      <c r="I39">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -3400,31 +3433,25 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E40">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F40">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G40">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H40">
-        <v>2</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="M40">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="I40">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -3438,48 +3465,45 @@
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E41">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="F41">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G41">
-        <v>12</v>
-      </c>
-      <c r="H41">
-        <v>12</v>
-      </c>
-      <c r="I41">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="L41">
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1">
-        <v>42886</v>
+        <v>42894</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F42">
-        <v>33</v>
-      </c>
-      <c r="G42">
-        <v>32</v>
-      </c>
-      <c r="L42">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -3493,19 +3517,16 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E43">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="F43">
-        <v>21</v>
-      </c>
-      <c r="H43">
-        <v>5</v>
-      </c>
-      <c r="I43">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="G43">
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -3516,19 +3537,22 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E44">
-        <v>60</v>
-      </c>
-      <c r="F44">
-        <v>14</v>
-      </c>
-      <c r="G44">
-        <v>19</v>
+        <v>90</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -3542,19 +3566,22 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E45">
         <v>90</v>
       </c>
+      <c r="F45">
+        <v>28</v>
+      </c>
+      <c r="G45">
+        <v>21</v>
+      </c>
       <c r="H45">
-        <v>4</v>
-      </c>
-      <c r="I45">
-        <v>9</v>
-      </c>
-      <c r="K45">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -3565,25 +3592,25 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E46">
         <v>90</v>
       </c>
       <c r="F46">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G46">
-        <v>21</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="M46">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="I46">
+        <v>9</v>
+      </c>
+      <c r="K46">
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -3597,22 +3624,19 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E47">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F47">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G47">
-        <v>13</v>
-      </c>
-      <c r="I47">
-        <v>9</v>
-      </c>
-      <c r="K47">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -3623,22 +3647,28 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E48">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F48">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G48">
-        <v>32</v>
-      </c>
-      <c r="J48">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>15</v>
+      </c>
+      <c r="I48">
+        <v>8</v>
+      </c>
+      <c r="K48">
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -3652,25 +3682,22 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E49">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F49">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49">
-        <v>15</v>
-      </c>
-      <c r="I49">
-        <v>8</v>
-      </c>
-      <c r="K49">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -3681,25 +3708,28 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E50">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F50">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="G50">
-        <v>27</v>
-      </c>
-      <c r="J50">
-        <v>2</v>
-      </c>
-      <c r="M50">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="H50">
+        <v>12</v>
+      </c>
+      <c r="I50">
+        <v>8</v>
+      </c>
+      <c r="K50">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -3713,25 +3743,22 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E51">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F51">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G51">
-        <v>6</v>
-      </c>
-      <c r="H51">
-        <v>12</v>
-      </c>
-      <c r="I51">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="K51">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -3742,25 +3769,25 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E52">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F52">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G52">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
       </c>
       <c r="K52">
-        <v>1</v>
-      </c>
-      <c r="M52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -3774,22 +3801,19 @@
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E53">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="F53">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G53">
-        <v>3</v>
-      </c>
-      <c r="I53">
-        <v>2</v>
-      </c>
-      <c r="K53">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -3800,21 +3824,27 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E54">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="F54">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G54">
-        <v>26</v>
-      </c>
-      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54">
+        <v>7</v>
+      </c>
+      <c r="K54">
         <v>1</v>
       </c>
     </row>
@@ -3829,25 +3859,19 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E55">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F55">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G55">
-        <v>4</v>
-      </c>
-      <c r="H55">
-        <v>5</v>
-      </c>
-      <c r="I55">
-        <v>7</v>
-      </c>
-      <c r="K55">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -3858,21 +3882,21 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E56">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F56">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="G56">
-        <v>24</v>
-      </c>
-      <c r="M56">
+        <v>12</v>
+      </c>
+      <c r="K56">
         <v>2</v>
       </c>
     </row>
@@ -3887,19 +3911,19 @@
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E57">
         <v>80</v>
       </c>
       <c r="F57">
+        <v>11</v>
+      </c>
+      <c r="G57">
         <v>16</v>
       </c>
-      <c r="G57">
-        <v>12</v>
-      </c>
-      <c r="K57">
-        <v>2</v>
+      <c r="M57">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -3910,22 +3934,28 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E58">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F58">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G58">
-        <v>16</v>
-      </c>
-      <c r="M58">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>6</v>
+      </c>
+      <c r="I58">
+        <v>9</v>
+      </c>
+      <c r="K58">
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -3939,25 +3969,16 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E59">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="F59">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G59">
-        <v>2</v>
-      </c>
-      <c r="H59">
-        <v>6</v>
-      </c>
-      <c r="I59">
-        <v>9</v>
-      </c>
-      <c r="K59">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -3968,19 +3989,25 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E60">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F60">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G60">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -3994,51 +4021,19 @@
         <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E61">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F61">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G61">
-        <v>5</v>
-      </c>
-      <c r="H61">
-        <v>5</v>
-      </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="1">
-        <v>42894</v>
-      </c>
-      <c r="B62">
-        <v>3</v>
-      </c>
-      <c r="C62">
-        <v>10</v>
-      </c>
-      <c r="D62" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62">
-        <v>80</v>
-      </c>
-      <c r="F62">
-        <v>17</v>
-      </c>
-      <c r="G62">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:M1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>